<commit_message>
Tourist Spot management system
</commit_message>
<xml_diff>
--- a/tourist_spot_management/Booking_Report.xlsx
+++ b/tourist_spot_management/Booking_Report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t>Booking ID</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>2024-06-07</t>
-  </si>
-  <si>
-    <t>confirmedd</t>
   </si>
   <si>
     <t>confirmed</t>
@@ -89,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -143,7 +140,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="n">
         <v>1.0</v>
@@ -158,7 +155,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" t="n">
         <v>100.5</v>
@@ -166,7 +163,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="n">
         <v>1.0</v>
@@ -181,7 +178,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" t="n">
         <v>100.5</v>
@@ -189,7 +186,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="n">
         <v>1.0</v>
@@ -204,7 +201,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" t="n">
         <v>100.5</v>
@@ -212,7 +209,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -227,7 +224,7 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="n">
         <v>100.5</v>
@@ -235,7 +232,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="n">
         <v>1.0</v>
@@ -250,78 +247,9 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" t="n">
-        <v>100.5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="n">
-        <v>100.5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="n">
-        <v>100.5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="n">
         <v>100.5</v>
       </c>
     </row>

</xml_diff>